<commit_message>
Changes to be committed: 	modified:   controladores/empresas.py 	modified:   controladores/exportar.py 	modified:   controladores/venda.py 	modified:   index.py 	new file:   static/arquivos_exportar/exportar.pdf 	modified:   static/arquivos_exportar/exportar.xlsx
</commit_message>
<xml_diff>
--- a/static/arquivos_exportar/exportar.xlsx
+++ b/static/arquivos_exportar/exportar.xlsx
@@ -327,7 +327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -371,15 +371,25 @@
       </c>
       <c r="G1" s="0" t="inlineStr">
         <is>
+          <t>Desconto</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>Desc. Uni.</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="J1" s="0" t="inlineStr">
         <is>
           <t>Data Venda</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="K1" s="0" t="inlineStr">
         <is>
           <t>Hora Venda</t>
         </is>
@@ -388,7 +398,7 @@
     <row r="2" ht="14.25" customHeight="1" s="3">
       <c r="A2" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -417,21 +427,27 @@
       <c r="G2" t="n">
         <v>100</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>08/02/2023</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>11:26:02.000</t>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>10:30:42.000</t>
         </is>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" s="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -455,19 +471,25 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>310.76</v>
+        <v>425.7</v>
       </c>
       <c r="G3" t="n">
-        <v>73</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>10/02/2023</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>13:38:40.000</t>
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>08/02/2023</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>09:45:15.000</t>
         </is>
       </c>
     </row>
@@ -503,12 +525,18 @@
       <c r="G4" t="n">
         <v>100</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>08/02/2023</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>11:00:39.000</t>
         </is>
@@ -517,7 +545,7 @@
     <row r="5" ht="14.25" customHeight="1" s="3">
       <c r="A5" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -541,26 +569,32 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>425.7</v>
+        <v>310.76</v>
       </c>
       <c r="G5" t="n">
-        <v>100</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>08/02/2023</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>09:45:15.000</t>
+        <v>73</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>73</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>10/02/2023</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>13:38:40.000</t>
         </is>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" s="3">
       <c r="A6" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -589,14 +623,20 @@
       <c r="G6" t="n">
         <v>100</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>100</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>08/02/2023</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>10:30:42.000</t>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>11:26:02.000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   controladores/clientes.py 	modified:   controladores/empresas.py 	modified:   controladores/usuarios.py 	modified:   controladores/vouchers.py 	modified:   index.py 	modified:   static/arquivos_exportar/exportar.pdf 	modified:   static/arquivos_exportar/exportar.xlsx
</commit_message>
<xml_diff>
--- a/static/arquivos_exportar/exportar.xlsx
+++ b/static/arquivos_exportar/exportar.xlsx
@@ -398,7 +398,7 @@
     <row r="2" ht="14.25" customHeight="1" s="3">
       <c r="A2" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -425,10 +425,10 @@
         <v>425.7</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
@@ -440,14 +440,14 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>10:30:42.000</t>
+          <t>09:45:15.000</t>
         </is>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" s="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -474,10 +474,10 @@
         <v>425.7</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>100</v>
@@ -489,7 +489,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09:45:15.000</t>
+          <t>10:30:42.000</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
     <row r="5" ht="14.25" customHeight="1" s="3">
       <c r="A5" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -569,32 +569,32 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>310.76</v>
+        <v>425.7</v>
       </c>
       <c r="G5" t="n">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>10/02/2023</t>
+          <t>08/02/2023</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>13:38:40.000</t>
+          <t>11:26:02.000</t>
         </is>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" s="3">
       <c r="A6" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -618,25 +618,25 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>425.7</v>
+        <v>310.76</v>
       </c>
       <c r="G6" t="n">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>08/02/2023</t>
+          <t>10/02/2023</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>11:26:02.000</t>
+          <t>13:38:40.000</t>
         </is>
       </c>
     </row>

</xml_diff>